<commit_message>
Added test cases and improved code
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\ICT3911Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94B2ADC-715A-45BE-A8B5-B6496859FFEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28857607-9DD1-4799-AC05-F24379D2C160}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="765" windowWidth="21600" windowHeight="10290" xr2:uid="{508BBE3A-2B24-4E7E-9ED8-96D293CDE31A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{508BBE3A-2B24-4E7E-9ED8-96D293CDE31A}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -70,19 +70,268 @@
     <t>Data</t>
   </si>
   <si>
-    <t>1. Edit data file and all sheets consistently</t>
-  </si>
-  <si>
     <t>Change data file completely whilst keeping the same format with consistent data</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>No errors and acceptable results</t>
-  </si>
-  <si>
     <t>The data entered was not representative of any real-life insturment panels</t>
+  </si>
+  <si>
+    <t>Repeat test 0 with new ideal k for clustering</t>
+  </si>
+  <si>
+    <t>The file needs to have been already run at least once with the new data.</t>
+  </si>
+  <si>
+    <t>More Accurate Clustering</t>
+  </si>
+  <si>
+    <t>1.Change k according to generated elbow-method graph. 2. Run file</t>
+  </si>
+  <si>
+    <t>No errors present and the results are accurate visualisations</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>No errors were found  and the visualisations worked as expected. The clustering was not accurate as the k of k-means needed to be changed - separate test</t>
+  </si>
+  <si>
+    <t>Run new data file and observe results</t>
+  </si>
+  <si>
+    <t>Add additional Attributes</t>
+  </si>
+  <si>
+    <t>1. Add extra attributes to datafile. 2. Run file</t>
+  </si>
+  <si>
+    <t>1. Edit data file and all sheets consistently by following the tempalte. 2. Format all sheets to text 3. Edit name of datafiles to be used to new data file</t>
+  </si>
+  <si>
+    <t>No errors present and the files are accepted</t>
+  </si>
+  <si>
+    <t>The files were accepted without error</t>
+  </si>
+  <si>
+    <t>1. Add data file to program. 2. Run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualisations </t>
+  </si>
+  <si>
+    <t>The attribute "Procedural Results" is not to be removed</t>
+  </si>
+  <si>
+    <t>Visualisations and clustering results reflected change</t>
+  </si>
+  <si>
+    <t>Visualisations and clustering reflect changes</t>
+  </si>
+  <si>
+    <t>Test Case 0 / A compliant data-file</t>
+  </si>
+  <si>
+    <t>Remove non-essential attributes</t>
+  </si>
+  <si>
+    <t>1. Remove attributes from QualitySheet. 2. Run</t>
+  </si>
+  <si>
+    <t>1_Result_final</t>
+  </si>
+  <si>
+    <t>0_Result_Final</t>
+  </si>
+  <si>
+    <t>0_Result_PanelInfo</t>
+  </si>
+  <si>
+    <t>0_Result_Procedures</t>
+  </si>
+  <si>
+    <t>0_TestData</t>
+  </si>
+  <si>
+    <t>1_EntireSequenceSheet</t>
+  </si>
+  <si>
+    <t>1_Result_PanelInfo</t>
+  </si>
+  <si>
+    <t>1_Result_Procedures</t>
+  </si>
+  <si>
+    <t>2_Before</t>
+  </si>
+  <si>
+    <t>2_Result</t>
+  </si>
+  <si>
+    <t>2_TestData</t>
+  </si>
+  <si>
+    <t>3_NewAttributeData</t>
+  </si>
+  <si>
+    <t>3_AttributeREsults</t>
+  </si>
+  <si>
+    <t>3_NewAttributeData_Clustering</t>
+  </si>
+  <si>
+    <t>3_newAttributeData_Radar</t>
+  </si>
+  <si>
+    <t>4_Clustering</t>
+  </si>
+  <si>
+    <t>4_RadarPlots</t>
+  </si>
+  <si>
+    <t>4_RemovedAttributes</t>
+  </si>
+  <si>
+    <t>4_RemovedAttributes_Graph</t>
+  </si>
+  <si>
+    <t>Partial Pass</t>
+  </si>
+  <si>
+    <t>Change order of numbers of procedures which use the same insturment multiple times</t>
+  </si>
+  <si>
+    <t>1. Swap multiple values in SequenceSheet and EntireSequenceSheet. E.g. 1,2 to 2,1</t>
+  </si>
+  <si>
+    <t>Script will crash in graph visualisations</t>
+  </si>
+  <si>
+    <t>Graphs did not crash, result was ideal</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Add Procedures in which insturments are used more than twice</t>
+  </si>
+  <si>
+    <t>Add non-existant instrument to SizeSpec</t>
+  </si>
+  <si>
+    <t>1. Add instrument and size specifications to table "SizeSpec"</t>
+  </si>
+  <si>
+    <t>No Difference in output</t>
+  </si>
+  <si>
+    <t>Add Procedures in which insturments are used more than twice and reverse order</t>
+  </si>
+  <si>
+    <t>1. Add new procedure in relevant tables. 2. Number order needs to use the same instrument more than two times. 3. Reverse sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add new procedure in relevant tables. 2. Number order needs to use the same instrument more than two times </t>
+  </si>
+  <si>
+    <t>This event should never occur, a user should never add any instrument that is not included in all other datasheets</t>
+  </si>
+  <si>
+    <t>Add instrument that is never used</t>
+  </si>
+  <si>
+    <t>1. Add instrument and size specifications to table "SizeSpec" and to all other sheets. 2. Set procedural use values to 0</t>
+  </si>
+  <si>
+    <t>Instrument will be only present in full graph but will not be connected.</t>
+  </si>
+  <si>
+    <t>Instrument was only present in full graph but was not connected.</t>
+  </si>
+  <si>
+    <t>5_EntireSequenceSheet_After</t>
+  </si>
+  <si>
+    <t>6_EntireSequenceSheet_After</t>
+  </si>
+  <si>
+    <t>7_EntireSequenceSheet_After</t>
+  </si>
+  <si>
+    <t>5_FinalGraph_After</t>
+  </si>
+  <si>
+    <t>5_FinalGraph_Before</t>
+  </si>
+  <si>
+    <t>5_Graph16_Before</t>
+  </si>
+  <si>
+    <t>5_SequenceSheet_After</t>
+  </si>
+  <si>
+    <t>5_Graph16_Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9_FinalGraph_Result_Before </t>
+  </si>
+  <si>
+    <t>6_EntireSequenceSheet_Before</t>
+  </si>
+  <si>
+    <t>6_FinalGraph_Result</t>
+  </si>
+  <si>
+    <t>6_PhaseSheet_After</t>
+  </si>
+  <si>
+    <t>6_PhaseSheet_Before</t>
+  </si>
+  <si>
+    <t>6_Procedure31_Result</t>
+  </si>
+  <si>
+    <t>6_SequenceSheet_After</t>
+  </si>
+  <si>
+    <t>6_SequenceSheet_Before</t>
+  </si>
+  <si>
+    <t>7_EntireSequenceSheet_Before</t>
+  </si>
+  <si>
+    <t>7_FinalGraph_Result_After</t>
+  </si>
+  <si>
+    <t>7_FinalGraph_Result_Before</t>
+  </si>
+  <si>
+    <t>7_Procedure31_After</t>
+  </si>
+  <si>
+    <t>7_Procedure31_Before</t>
+  </si>
+  <si>
+    <t>7_SequenceSheet_After</t>
+  </si>
+  <si>
+    <t>7_SequenceSheet_Before</t>
+  </si>
+  <si>
+    <t>8_SizeSpec_After</t>
+  </si>
+  <si>
+    <t>8_SizeSpec_Before</t>
+  </si>
+  <si>
+    <t>9_FinalGraph_Result_After</t>
   </si>
 </sst>
 </file>
@@ -209,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -226,6 +475,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D1A8C3-E998-452B-86FC-DCE7FC13ECCC}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,15 +804,16 @@
     <col min="1" max="1" width="2.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="6" customWidth="1"/>
     <col min="7" max="7" width="27.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -588,8 +841,11 @@
       <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -600,19 +856,292 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="J2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="E4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>16</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -622,18 +1151,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F62351-99CA-4E5B-96C4-683DB3E45CC3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,10 +1178,416 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Set to presentable and final
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\ICT3911Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9941E3B-2B4E-42FD-AA14-3C438C72C507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA855AFC-D679-4403-BBFF-F94C4E338457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{508BBE3A-2B24-4E7E-9ED8-96D293CDE31A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="120">
   <si>
     <t>ID</t>
   </si>
@@ -383,6 +383,15 @@
   </si>
   <si>
     <t>Instrument was only present in full graph but was not connected. It is present in the Legend and in all of  the results.</t>
+  </si>
+  <si>
+    <t>Results reflected changes as expected and on graphs</t>
+  </si>
+  <si>
+    <t>Clustering results reflected change as edge weights had less values</t>
+  </si>
+  <si>
+    <t>Ideally an insturment is used in at least one procedure.</t>
   </si>
 </sst>
 </file>
@@ -860,7 +869,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1461,9 @@
       <c r="H19" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="J19" s="9" t="s">
         <v>55</v>
       </c>
@@ -1477,13 +1488,15 @@
       <c r="G20" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>112</v>
+      <c r="H20" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J20" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1505,13 +1518,15 @@
       <c r="G21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="12" t="s">
-        <v>31</v>
+      <c r="H21" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3">

</xml_diff>